<commit_message>
feat: Update LinkedIn automation workflow for outreach and messaging
</commit_message>
<xml_diff>
--- a/inb/linkedin-data.xlsx
+++ b/inb/linkedin-data.xlsx
@@ -478,12 +478,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>connect_sent</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Expected any one of public_id or urn_id</t>
+          <t>2026-02-06 10:26:38.535002</t>
         </is>
       </c>
     </row>
@@ -505,12 +505,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>error</t>
+          <t>connect_sent</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Expected any one of public_id or urn_id</t>
+          <t>2026-02-06 10:27:08.959432</t>
         </is>
       </c>
     </row>
@@ -792,8 +792,16 @@
           <t>Tenstorrent Inc.</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>no_connect_button</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -811,8 +819,16 @@
           <t>Headout</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>error: Message: invalid session id: session delete</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">

</xml_diff>